<commit_message>
Inclusao de novos campos na linha de imovel para o recadastramento
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Retorno.xlsx
+++ b/recadastramento/layout/Layout_Retorno.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="0" windowWidth="16400" windowHeight="8200" tabRatio="657" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24920" windowHeight="15540" tabRatio="657" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="Hidrômetro" sheetId="6" r:id="rId6"/>
     <sheet name="Anormalidade Imovel" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="170">
   <si>
     <t>linha tipo 00</t>
   </si>
@@ -636,12 +636,78 @@
   <si>
     <t>Usuário, Proprietário, Responsável, Parente, Funcionário</t>
   </si>
+  <si>
+    <t>area_construida</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
+  <si>
+    <t>classe_social</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>1 - Alta | 2 - Media | 3 - Baixa | 4 - Sub</t>
+  </si>
+  <si>
+    <t>quantidade_animais_domesticos</t>
+  </si>
+  <si>
+    <t>vol_cisterna</t>
+  </si>
+  <si>
+    <t>vol_piscina</t>
+  </si>
+  <si>
+    <t>vol_cx_dagua</t>
+  </si>
+  <si>
+    <t>tipo_uso</t>
+  </si>
+  <si>
+    <t>1 - dormitorio | 2 - morada | 3 - veraneio | 4 - outros</t>
+  </si>
+  <si>
+    <t>acesso_hidrometro</t>
+  </si>
+  <si>
+    <t>1 - bom | 2 - ruim | 3 - sem</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Crianças</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Adultos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Idosos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Empregados</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Alunos</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Cães</t>
+  </si>
+  <si>
+    <t>Tipo de ocupante: Outros</t>
+  </si>
+  <si>
+    <t>quantidade_economias_social</t>
+  </si>
+  <si>
+    <t>quantidade_economias_outros</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -697,8 +763,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -715,6 +797,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -742,10 +830,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -811,11 +901,20 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1216,7 +1315,7 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2332,10 +2431,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H42"/>
+  <dimension ref="B1:H59"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2390,7 +2489,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" ref="D4:D42" si="0">SUM(C3,D3)</f>
+        <f t="shared" ref="D4:D59" si="0">SUM(C3,D3)</f>
         <v>3</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -2398,7 +2497,7 @@
       </c>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="2:6" s="15" customFormat="1" ht="31.25" customHeight="1">
+    <row r="5" spans="2:6" s="15" customFormat="1">
       <c r="B5" s="16" t="s">
         <v>82</v>
       </c>
@@ -2430,7 +2529,7 @@
       <c r="E6" s="9"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="2:6" s="15" customFormat="1" ht="31.25" customHeight="1">
+    <row r="7" spans="2:6" s="15" customFormat="1">
       <c r="B7" s="19" t="s">
         <v>85</v>
       </c>
@@ -2560,7 +2659,7 @@
       </c>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" spans="2:6" ht="31.25" customHeight="1">
+    <row r="15" spans="2:6">
       <c r="B15" s="19" t="s">
         <v>93</v>
       </c>
@@ -2965,57 +3064,345 @@
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="17" customHeight="1">
-      <c r="B40" s="4" t="s">
+    <row r="40" spans="2:8">
+      <c r="B40" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" s="30">
+        <v>10</v>
+      </c>
+      <c r="D40" s="30">
+        <f t="shared" si="0"/>
+        <v>307</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="31">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="30">
+        <v>1</v>
+      </c>
+      <c r="D41" s="30">
+        <f t="shared" si="0"/>
+        <v>317</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C42" s="30">
+        <v>4</v>
+      </c>
+      <c r="D42" s="30">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+      <c r="E42" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="29"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="C43" s="30">
+        <v>7</v>
+      </c>
+      <c r="D43" s="30">
+        <f t="shared" si="0"/>
+        <v>322</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="31">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C44" s="30">
+        <v>7</v>
+      </c>
+      <c r="D44" s="30">
+        <f t="shared" si="0"/>
+        <v>329</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F44" s="31">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C45" s="30">
+        <v>7</v>
+      </c>
+      <c r="D45" s="30">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>149</v>
+      </c>
+      <c r="F45" s="31">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="C46" s="30">
+        <v>1</v>
+      </c>
+      <c r="D46" s="30">
+        <f t="shared" si="0"/>
+        <v>343</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="C47" s="30">
+        <v>1</v>
+      </c>
+      <c r="D47" s="30">
+        <f t="shared" si="0"/>
+        <v>344</v>
+      </c>
+      <c r="E47" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8">
+      <c r="B48" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="30">
+        <v>4</v>
+      </c>
+      <c r="D48" s="30">
+        <f t="shared" si="0"/>
+        <v>345</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="29"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="30">
+        <v>4</v>
+      </c>
+      <c r="D49" s="30">
+        <f t="shared" si="0"/>
+        <v>349</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="C50" s="30">
+        <v>4</v>
+      </c>
+      <c r="D50" s="30">
+        <f t="shared" si="0"/>
+        <v>353</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="29"/>
+    </row>
+    <row r="51" spans="2:8">
+      <c r="B51" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="30">
+        <v>4</v>
+      </c>
+      <c r="D51" s="30">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="29"/>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C52" s="30">
+        <v>4</v>
+      </c>
+      <c r="D52" s="30">
+        <f t="shared" si="0"/>
+        <v>361</v>
+      </c>
+      <c r="E52" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="29"/>
+    </row>
+    <row r="53" spans="2:8">
+      <c r="B53" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" s="30">
+        <v>4</v>
+      </c>
+      <c r="D53" s="30">
+        <f t="shared" si="0"/>
+        <v>365</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="29"/>
+    </row>
+    <row r="54" spans="2:8">
+      <c r="B54" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" s="30">
+        <v>4</v>
+      </c>
+      <c r="D54" s="30">
+        <f t="shared" si="0"/>
+        <v>369</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="29"/>
+    </row>
+    <row r="55" spans="2:8">
+      <c r="B55" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C55" s="30">
+        <v>3</v>
+      </c>
+      <c r="D55" s="30">
+        <f t="shared" si="0"/>
+        <v>373</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="29"/>
+      <c r="H55" s="21"/>
+    </row>
+    <row r="56" spans="2:8">
+      <c r="B56" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="C56" s="30">
+        <v>3</v>
+      </c>
+      <c r="D56" s="30">
+        <f t="shared" si="0"/>
+        <v>376</v>
+      </c>
+      <c r="E56" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="29"/>
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="2:8" ht="17" customHeight="1">
+      <c r="B57" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C57" s="5">
         <v>20</v>
       </c>
-      <c r="D40" s="5">
-        <f t="shared" si="0"/>
-        <v>307</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="4"/>
-    </row>
-    <row r="41" spans="2:8" ht="17" customHeight="1">
-      <c r="B41" s="4" t="s">
+      <c r="D57" s="5">
+        <f t="shared" si="0"/>
+        <v>379</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="2:8" ht="17" customHeight="1">
+      <c r="B58" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C58" s="5">
         <v>20</v>
       </c>
-      <c r="D41" s="5">
-        <f t="shared" si="0"/>
-        <v>327</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="4"/>
-    </row>
-    <row r="42" spans="2:8" ht="17" customHeight="1">
-      <c r="B42" s="4" t="s">
+      <c r="D58" s="5">
+        <f t="shared" si="0"/>
+        <v>399</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="2:8" ht="17" customHeight="1">
+      <c r="B59" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C59" s="6">
         <v>26</v>
       </c>
-      <c r="D42" s="5">
-        <f t="shared" si="0"/>
-        <v>347</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="D59" s="5">
+        <f t="shared" si="0"/>
+        <v>419</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="14"/>
+      <c r="F59" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.51180555555555496" right="0.51180555555555496" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3028,7 +3415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3110,13 +3497,13 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="45.5" customHeight="1">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Incremento do tamanho dos telefones no layout
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Retorno.xlsx
+++ b/recadastramento/layout/Layout_Retorno.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24920" windowHeight="15540" tabRatio="657" activeTab="2"/>
+    <workbookView xWindow="-2500" yWindow="-18000" windowWidth="28800" windowHeight="17540" tabRatio="657" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F56"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1759,7 +1759,7 @@
         <v>38</v>
       </c>
       <c r="C17" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" si="0"/>
@@ -1777,11 +1777,11 @@
         <v>40</v>
       </c>
       <c r="C18" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
@@ -1799,7 +1799,7 @@
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="D20" s="5">
         <f t="shared" si="0"/>
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>19</v>
@@ -1831,7 +1831,7 @@
       </c>
       <c r="D21" s="5">
         <f t="shared" si="0"/>
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
@@ -1847,7 +1847,7 @@
       </c>
       <c r="D22" s="5">
         <f t="shared" si="0"/>
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>19</v>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="D23" s="5">
         <f t="shared" si="0"/>
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="D24" s="5">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
@@ -1897,7 +1897,7 @@
       </c>
       <c r="D25" s="5">
         <f t="shared" si="0"/>
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
@@ -1913,7 +1913,7 @@
       </c>
       <c r="D26" s="5">
         <f t="shared" si="0"/>
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>19</v>
@@ -1927,11 +1927,11 @@
         <v>49</v>
       </c>
       <c r="C27" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D27" s="5">
         <f t="shared" si="0"/>
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
@@ -1945,11 +1945,11 @@
         <v>50</v>
       </c>
       <c r="C28" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D28" s="5">
         <f t="shared" si="0"/>
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
@@ -1967,7 +1967,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" si="0"/>
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>9</v>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="D30" s="5">
         <f t="shared" si="0"/>
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>19</v>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="D31" s="5">
         <f t="shared" si="0"/>
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>9</v>
@@ -2017,7 +2017,7 @@
       </c>
       <c r="D32" s="5">
         <f t="shared" si="0"/>
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>9</v>
@@ -2033,7 +2033,7 @@
       </c>
       <c r="D33" s="5">
         <f t="shared" si="0"/>
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>9</v>
@@ -2049,7 +2049,7 @@
       </c>
       <c r="D34" s="5">
         <f t="shared" si="0"/>
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>9</v>
@@ -2065,7 +2065,7 @@
       </c>
       <c r="D35" s="5">
         <f t="shared" si="0"/>
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>19</v>
@@ -2081,7 +2081,7 @@
       </c>
       <c r="D36" s="5">
         <f t="shared" ref="D36:D56" si="1">SUM(C35,D35)</f>
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>9</v>
@@ -2097,7 +2097,7 @@
       </c>
       <c r="D37" s="5">
         <f t="shared" si="1"/>
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>19</v>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="D38" s="5">
         <f t="shared" si="1"/>
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>9</v>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="D39" s="5">
         <f t="shared" si="1"/>
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>19</v>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="D40" s="5">
         <f t="shared" si="1"/>
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>9</v>
@@ -2163,7 +2163,7 @@
       </c>
       <c r="D41" s="5">
         <f t="shared" si="1"/>
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>9</v>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D42" s="5">
         <f t="shared" si="1"/>
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>9</v>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="D43" s="5">
         <f t="shared" si="1"/>
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>19</v>
@@ -2209,11 +2209,11 @@
         <v>67</v>
       </c>
       <c r="C44" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D44" s="5">
         <f t="shared" si="1"/>
-        <v>514</v>
+        <v>518</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>9</v>
@@ -2227,11 +2227,11 @@
         <v>68</v>
       </c>
       <c r="C45" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D45" s="5">
         <f t="shared" si="1"/>
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>9</v>
@@ -2249,7 +2249,7 @@
       </c>
       <c r="D46" s="5">
         <f t="shared" si="1"/>
-        <v>534</v>
+        <v>540</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>9</v>
@@ -2265,7 +2265,7 @@
       </c>
       <c r="D47" s="5">
         <f t="shared" si="1"/>
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>19</v>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="D48" s="5">
         <f t="shared" si="1"/>
-        <v>566</v>
+        <v>572</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>9</v>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="D49" s="5">
         <f t="shared" si="1"/>
-        <v>606</v>
+        <v>612</v>
       </c>
       <c r="E49" s="5" t="s">
         <v>9</v>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="D50" s="5">
         <f t="shared" si="1"/>
-        <v>611</v>
+        <v>617</v>
       </c>
       <c r="E50" s="5" t="s">
         <v>9</v>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="D51" s="5">
         <f t="shared" si="1"/>
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="E51" s="5" t="s">
         <v>9</v>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D52" s="5">
         <f t="shared" si="1"/>
-        <v>656</v>
+        <v>662</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>19</v>
@@ -2363,7 +2363,7 @@
       </c>
       <c r="D53" s="5">
         <f t="shared" si="1"/>
-        <v>664</v>
+        <v>670</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>9</v>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="D54" s="5">
         <f t="shared" si="1"/>
-        <v>679</v>
+        <v>685</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>9</v>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="D55" s="5">
         <f t="shared" si="1"/>
-        <v>699</v>
+        <v>705</v>
       </c>
       <c r="E55" s="5" t="s">
         <v>9</v>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="D56" s="5">
         <f t="shared" si="1"/>
-        <v>719</v>
+        <v>725</v>
       </c>
       <c r="E56" s="5" t="s">
         <v>80</v>
@@ -2433,8 +2433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Atualizacao do layout de retorno
</commit_message>
<xml_diff>
--- a/recadastramento/layout/Layout_Retorno.xlsx
+++ b/recadastramento/layout/Layout_Retorno.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-880" yWindow="-18000" windowWidth="26160" windowHeight="17080" tabRatio="657" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24900" windowHeight="15600" tabRatio="657" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cabeçalho" sheetId="1" r:id="rId1"/>
@@ -917,15 +917,15 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3361,19 +3361,20 @@
       <c r="H56" s="21"/>
     </row>
     <row r="57" spans="2:8">
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="C57" s="34">
+      <c r="C57" s="33">
         <v>3</v>
       </c>
-      <c r="D57" s="34">
-        <v>378</v>
-      </c>
-      <c r="E57" s="34" t="s">
+      <c r="D57" s="30">
+        <f t="shared" si="0"/>
+        <v>379</v>
+      </c>
+      <c r="E57" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="F57" s="35" t="s">
+      <c r="F57" s="34" t="s">
         <v>170</v>
       </c>
       <c r="H57" s="21"/>
@@ -3386,8 +3387,8 @@
         <v>20</v>
       </c>
       <c r="D58" s="5">
-        <f>SUM(C56,D56)</f>
-        <v>379</v>
+        <f t="shared" si="0"/>
+        <v>382</v>
       </c>
       <c r="E58" s="5" t="s">
         <v>9</v>
@@ -3403,7 +3404,7 @@
       </c>
       <c r="D59" s="5">
         <f t="shared" si="0"/>
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="E59" s="5" t="s">
         <v>9</v>
@@ -3419,7 +3420,7 @@
       </c>
       <c r="D60" s="5">
         <f t="shared" si="0"/>
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E60" s="5" t="s">
         <v>77</v>
@@ -3523,13 +3524,13 @@
       </c>
     </row>
     <row r="7" spans="2:6" ht="45.5" customHeight="1">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>